<commit_message>
add new code and test case for plotting
</commit_message>
<xml_diff>
--- a/test/List of Tests.xlsx
+++ b/test/List of Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="96" windowWidth="19752" windowHeight="9204"/>
+    <workbookView xWindow="192" yWindow="156" windowWidth="19752" windowHeight="9144"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Description</t>
   </si>
@@ -22,17 +22,7 @@
     <t>Check if input files exists</t>
   </si>
   <si>
-    <t>Check if output structure is correctly set</t>
-  </si>
-  <si>
     <t>expected outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breaks with logfile message
- 25-Jul-2017 14:15:42 ERROR: Outputpath "Organism|PeripheralVenousBlood|Hydroxy_Itraconazole|Plasma (Peripheral Venous Blood)_withTypo" could not be found in model
-25-Jul-2017 14:15:42 ERROR: output Organism|PeripheralVenousBlood|Itraconazole|Plasma (Peripheral Venous Blood) has unit "µmol/l", there is no common dimension with display unit "cm"
-25-Jul-2017 14:15:42 ERROR: unit "Organism|PeripheralVenousBlood|Midazolam|Plasma (Peripheral Venous Blood)" for "Typo" seems to be no default OSPSuite unit
-</t>
   </si>
   <si>
     <t>Breaks with logfile message 
@@ -41,17 +31,11 @@
 25-Jul-2017 13:36:56 ERROR: "Children_OralSingle_IV_Multi_withTypo.csv " does not exist</t>
   </si>
   <si>
-    <t>Population simulation and PK Parameter caluclation of a multi application</t>
-  </si>
-  <si>
     <t>Two csv files are generated: 
 Simulations/OralSingle_IV_Multi-PK-Analyses.csv
 Simulations/OralSingle_IV_Multi-Results.csv</t>
   </si>
   <si>
-    <t>Populations simulation with studydesign.csv</t>
-  </si>
-  <si>
     <t>Models</t>
   </si>
   <si>
@@ -80,13 +64,41 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Two csv files are generated: 
+simulations/SingleIvBolus-Results.csv
+simulations/SingleIvBolus-PK-Analyses.csv</t>
+  </si>
+  <si>
+    <t>Find inconsitencies in output cvs</t>
+  </si>
+  <si>
+    <t>Breaks with logfile message
+ERROR: Outputpath "Organism|PeripheralVenousBlood|Hydroxy_Itraconazole|Plasma (Peripheral Venous Blood) with Typo" could not be found in model
+ERROR: For unit "µmol/l", there is no common dimension with display unit "cm"
+ERROR: unit "typo" for seems to be no default OSPSuite unit
+ERROR: unit "typo2" for seems to be no default OSPSuite unit
+ERROR: For unit "µmol/l", there is no common dimension with display unit "h"</t>
+  </si>
+  <si>
+    <t>Population simulation and PK Parameter calculation of a multi application</t>
+  </si>
+  <si>
+    <t>7.2_BSA_Example</t>
+  </si>
+  <si>
+    <t>Populations simulation with studydesign.csv dose per bodyweigth</t>
+  </si>
+  <si>
+    <t>Populations simulation with studydesign.csv dose per surface area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +108,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -126,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -135,6 +152,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.3984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -456,19 +476,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="82.8" x14ac:dyDescent="0.25">
@@ -479,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -490,21 +510,24 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -512,29 +535,38 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -542,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -550,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,7 +590,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -566,7 +598,12 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>